<commit_message>
worked on enchantment formulas, and on diagrams of various emission areas.
</commit_message>
<xml_diff>
--- a/Enchantments/Items/Uncommon.xlsx
+++ b/Enchantments/Items/Uncommon.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842B7550-F60A-4AF5-BBA2-3179344FBB6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E8BB49-34AD-4756-9106-32B583F91B7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Berserker" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Uncommon</t>
   </si>
@@ -270,15 +270,9 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> · Medium diamond (+3 MCI for forcebinding)</t>
-  </si>
-  <si>
     <t>3RD-LEVEL MAGIC WEAPON</t>
   </si>
   <si>
-    <t xml:space="preserve"> · Small sunstone (+2 MCI for spiritual weapon)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Enchanted </t>
     </r>
@@ -321,29 +315,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> · Medium ruby (3d6 fire </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>→</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 3d10 fire)</t>
     </r>
   </si>
   <si>
@@ -962,7 +933,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1018,12 +989,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1092,7 +1057,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1141,36 +1106,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1184,11 +1125,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1201,38 +1153,31 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1519,10 +1464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91708881-980A-49CF-9BC2-CEDE7A37C7A6}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1532,70 +1477,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="17"/>
+      <c r="A1" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="B5" s="20"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="14"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="22"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1603,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54EB7FB-9D42-476B-9E36-E5C9019CDADC}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,96 +1551,82 @@
     <col min="1" max="2" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="12"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="13"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="B1" s="20"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B2" s="21" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="20"/>
+    </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="12"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="13"/>
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>7</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>3</v>
+        <v>29</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>32</v>
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1711,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA7491C-8F44-48E8-8AD9-55CBF99A4954}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,64 +1645,57 @@
     <col min="1" max="2" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="12"/>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="16"/>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="20"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1788,10 +1704,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E885A785-C60D-46A5-A4BF-3A3D889E2C11}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,84 +1717,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="17"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="18"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="15"/>
+      <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="14"/>
+        <v>23</v>
+      </c>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>